<commit_message>
[ADD] ATP tuning; Registering analysis
</commit_message>
<xml_diff>
--- a/environmental_conditions/carbon_sources_conditions.xlsx
+++ b/environmental_conditions/carbon_sources_conditions.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Pycharm_projects/lab_models/environmental_conditions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="127" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B57F1050-E891-46CA-91EC-808E690E8B5C}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A946286E-A4DF-4524-B6C5-7DF1488BC200}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
   </bookViews>
   <sheets>
-    <sheet name="iCC431" sheetId="1" r:id="rId1"/>
+    <sheet name="iCC390" sheetId="2" r:id="rId1"/>
+    <sheet name="iCC431" sheetId="1" r:id="rId2"/>
+    <sheet name="iCC464" sheetId="3" r:id="rId3"/>
+    <sheet name="iCC644" sheetId="4" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iCC464'!$A$1:$B$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="214">
   <si>
     <t>exchange</t>
   </si>
@@ -111,9 +117,6 @@
     <t>EX_leu__L_e</t>
   </si>
   <si>
-    <t>EX_glu__L__e</t>
-  </si>
-  <si>
     <t>EX_phe__L_e</t>
   </si>
   <si>
@@ -454,6 +457,231 @@
   </si>
   <si>
     <t>EX_cbasp_e</t>
+  </si>
+  <si>
+    <t>EX_glu__L_e</t>
+  </si>
+  <si>
+    <t>EX_nac_e</t>
+  </si>
+  <si>
+    <t>EX_ocdca_e</t>
+  </si>
+  <si>
+    <t>EX_thym_e</t>
+  </si>
+  <si>
+    <t>EX_tre_e</t>
+  </si>
+  <si>
+    <t>EX_hdca_e</t>
+  </si>
+  <si>
+    <t>EX_tetdecacid_e</t>
+  </si>
+  <si>
+    <t>EX_ch4s_e</t>
+  </si>
+  <si>
+    <t>EX_orot_e</t>
+  </si>
+  <si>
+    <t>EX_mththf_e</t>
+  </si>
+  <si>
+    <t>EX_hqn_e</t>
+  </si>
+  <si>
+    <t>EX_hexedecacid_e</t>
+  </si>
+  <si>
+    <t>EX_cit_e</t>
+  </si>
+  <si>
+    <t>EX_a_gal__D_e</t>
+  </si>
+  <si>
+    <t>EX_malt_e</t>
+  </si>
+  <si>
+    <t>EX_2hymeph_e</t>
+  </si>
+  <si>
+    <t>EX_gal_bD_e</t>
+  </si>
+  <si>
+    <t>EX_salcn_e</t>
+  </si>
+  <si>
+    <t>EX_arbt_e</t>
+  </si>
+  <si>
+    <t>EX_lac__D_e</t>
+  </si>
+  <si>
+    <t>EX_ocdcea_e</t>
+  </si>
+  <si>
+    <t>EX_2hbut_e</t>
+  </si>
+  <si>
+    <t>EX_cmp_e</t>
+  </si>
+  <si>
+    <t>EX_amp_e</t>
+  </si>
+  <si>
+    <t>EX_so2_e</t>
+  </si>
+  <si>
+    <t>EX_mal__L_e</t>
+  </si>
+  <si>
+    <t>EX_co_e</t>
+  </si>
+  <si>
+    <t>EX_pydam_e</t>
+  </si>
+  <si>
+    <t>EX_raffin_e</t>
+  </si>
+  <si>
+    <t>EX_3ump_e</t>
+  </si>
+  <si>
+    <t>EX_acgam_e</t>
+  </si>
+  <si>
+    <t>EX_acmum_e</t>
+  </si>
+  <si>
+    <t>EX_C16639_e</t>
+  </si>
+  <si>
+    <t>EX_melib_e</t>
+  </si>
+  <si>
+    <t>EX_3cmp_e</t>
+  </si>
+  <si>
+    <t>EX_3gmp_e</t>
+  </si>
+  <si>
+    <t>EX_oxa_e</t>
+  </si>
+  <si>
+    <t>EX_glyclt_e</t>
+  </si>
+  <si>
+    <t>EX_pydxn_e</t>
+  </si>
+  <si>
+    <t>EX_3amp_e</t>
+  </si>
+  <si>
+    <t>EX_isomal_e</t>
+  </si>
+  <si>
+    <t>EX_stys_e</t>
+  </si>
+  <si>
+    <t>EX_4abut_e</t>
+  </si>
+  <si>
+    <t>EX_cbl1_e</t>
+  </si>
+  <si>
+    <t>EX_tag__D_e</t>
+  </si>
+  <si>
+    <t>EX_2pg_e</t>
+  </si>
+  <si>
+    <t>EX_mnl_e</t>
+  </si>
+  <si>
+    <t>EX_C01019_e</t>
+  </si>
+  <si>
+    <t>EX_3pg_e</t>
+  </si>
+  <si>
+    <t>EX_fruur_e</t>
+  </si>
+  <si>
+    <t>EX_d5kgp_e</t>
+  </si>
+  <si>
+    <t>EX_sbt__D_e</t>
+  </si>
+  <si>
+    <t>EX_HC00822_e</t>
+  </si>
+  <si>
+    <t>EX_glcur_e</t>
+  </si>
+  <si>
+    <t>EX_alaala_e</t>
+  </si>
+  <si>
+    <t>EX_mana_e</t>
+  </si>
+  <si>
+    <t>EX_asp__D_e</t>
+  </si>
+  <si>
+    <t>EX_srb__L_e</t>
+  </si>
+  <si>
+    <t>EX_xylt_e</t>
+  </si>
+  <si>
+    <t>EX_lald__L_e</t>
+  </si>
+  <si>
+    <t>EX_13dpg_e</t>
+  </si>
+  <si>
+    <t>EX_rmn_e</t>
+  </si>
+  <si>
+    <t>EX_C00072_e</t>
+  </si>
+  <si>
+    <t>EX_mthgxl_e</t>
+  </si>
+  <si>
+    <t>EX_C00261_e</t>
+  </si>
+  <si>
+    <t>EX_C01326_e</t>
+  </si>
+  <si>
+    <t>EX_C03912_e</t>
+  </si>
+  <si>
+    <t>EX_glcn__D_e</t>
+  </si>
+  <si>
+    <t>EX_HC00832_e</t>
+  </si>
+  <si>
+    <t>EX_inost_e</t>
+  </si>
+  <si>
+    <t>EX_C07086_e</t>
+  </si>
+  <si>
+    <t>EX_galt_e</t>
+  </si>
+  <si>
+    <t>EX_C00819_e</t>
+  </si>
+  <si>
+    <t>EX_4h2oxg_e</t>
+  </si>
+  <si>
+    <t>EX_C16737_e</t>
   </si>
 </sst>
 </file>
@@ -813,11 +1041,642 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05448E04-8BCE-4735-A6A7-A6D273D113C3}">
+  <dimension ref="A1:B77"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B11">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>35</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>159</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>23</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>141</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>27</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>156</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>19</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>145</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>147</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>155</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>148</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>149</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>84</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>150</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>77</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>151</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>93</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>142</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>61</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>152</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>112</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>61</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F2E160-0E44-4C80-A334-F20DED143A47}">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1020,7 +1879,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="B25">
         <v>1</v>
@@ -1028,7 +1887,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -1036,7 +1895,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -1044,7 +1903,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -1052,7 +1911,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -1060,7 +1919,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -1068,7 +1927,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -1076,7 +1935,1134 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>32</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>90</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>91</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>92</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>93</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>95</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>101</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>103</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>105</v>
+      </c>
+      <c r="B106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>106</v>
+      </c>
+      <c r="B107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>107</v>
+      </c>
+      <c r="B108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>108</v>
+      </c>
+      <c r="B109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>109</v>
+      </c>
+      <c r="B110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>110</v>
+      </c>
+      <c r="B111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>111</v>
+      </c>
+      <c r="B112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>112</v>
+      </c>
+      <c r="B113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>113</v>
+      </c>
+      <c r="B114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>114</v>
+      </c>
+      <c r="B115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>115</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>116</v>
+      </c>
+      <c r="B117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
+        <v>118</v>
+      </c>
+      <c r="B119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
+        <v>119</v>
+      </c>
+      <c r="B120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
+        <v>120</v>
+      </c>
+      <c r="B121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A122" t="s">
+        <v>121</v>
+      </c>
+      <c r="B122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A123" t="s">
+        <v>122</v>
+      </c>
+      <c r="B123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>123</v>
+      </c>
+      <c r="B124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A125" t="s">
+        <v>124</v>
+      </c>
+      <c r="B125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A126" t="s">
+        <v>125</v>
+      </c>
+      <c r="B126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A127" t="s">
+        <v>126</v>
+      </c>
+      <c r="B127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A128" t="s">
+        <v>127</v>
+      </c>
+      <c r="B128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>128</v>
+      </c>
+      <c r="B129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A130" t="s">
+        <v>129</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A131" t="s">
+        <v>130</v>
+      </c>
+      <c r="B131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>131</v>
+      </c>
+      <c r="B132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A133" t="s">
+        <v>132</v>
+      </c>
+      <c r="B133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A134" t="s">
+        <v>133</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A135" t="s">
+        <v>134</v>
+      </c>
+      <c r="B135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>135</v>
+      </c>
+      <c r="B136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>136</v>
+      </c>
+      <c r="B137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A138" t="s">
+        <v>137</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
+        <v>138</v>
+      </c>
+      <c r="B139">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1127718F-E99E-4924-AB7E-48BFF007017E}">
+  <dimension ref="A1:B105"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B13">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>159</v>
+      </c>
+      <c r="B15">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>141</v>
+      </c>
+      <c r="B20">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B23">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>31</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -1092,7 +3078,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -1100,7 +3086,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1108,7 +3094,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1116,7 +3102,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1124,7 +3110,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1132,7 +3118,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B39">
         <v>1</v>
@@ -1140,7 +3126,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1148,7 +3134,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>139</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -1164,15 +3150,15 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>43</v>
+        <v>164</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>44</v>
+        <v>175</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -1180,15 +3166,15 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>46</v>
+      <c r="A46" t="s">
+        <v>20</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -1196,7 +3182,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -1204,15 +3190,15 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>48</v>
+        <v>180</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>49</v>
+      <c r="A49" t="s">
+        <v>96</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -1220,7 +3206,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>151</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -1228,7 +3214,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -1236,7 +3222,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>176</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -1244,7 +3230,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -1252,7 +3238,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>54</v>
+        <v>156</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -1260,23 +3246,23 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
       <c r="B55">
         <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="1" t="s">
-        <v>56</v>
+      <c r="A56" t="s">
+        <v>48</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
-        <v>57</v>
+      <c r="A57" t="s">
+        <v>165</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -1284,7 +3270,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -1292,31 +3278,31 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>59</v>
+        <v>166</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="1" t="s">
-        <v>60</v>
+      <c r="A60" t="s">
+        <v>172</v>
       </c>
       <c r="B60">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="1" t="s">
-        <v>61</v>
+      <c r="A61" t="s">
+        <v>153</v>
       </c>
       <c r="B61">
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="1" t="s">
-        <v>62</v>
+      <c r="A62" t="s">
+        <v>178</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -1324,15 +3310,15 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
-        <v>64</v>
+      <c r="A64" t="s">
+        <v>90</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -1340,7 +3326,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>65</v>
+        <v>181</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -1348,7 +3334,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>66</v>
+        <v>143</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -1356,7 +3342,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -1364,7 +3350,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>68</v>
+        <v>154</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -1372,7 +3358,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -1380,7 +3366,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -1388,7 +3374,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>71</v>
+        <v>160</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -1396,7 +3382,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -1404,7 +3390,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -1412,7 +3398,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -1420,7 +3406,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -1428,7 +3414,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -1436,7 +3422,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -1444,7 +3430,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -1452,7 +3438,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>79</v>
+        <v>163</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -1460,7 +3446,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>80</v>
+        <v>13</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -1468,7 +3454,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>81</v>
+        <v>155</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -1476,15 +3462,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>82</v>
+        <v>148</v>
       </c>
       <c r="B82">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>83</v>
+      <c r="A83" t="s">
+        <v>57</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -1492,7 +3478,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -1500,7 +3486,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -1508,15 +3494,15 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>86</v>
+        <v>179</v>
       </c>
       <c r="B86">
         <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>87</v>
+      <c r="A87" t="s">
+        <v>17</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -1524,7 +3510,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -1532,7 +3518,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -1540,7 +3526,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>90</v>
+        <v>173</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -1548,7 +3534,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -1556,7 +3542,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>92</v>
+        <v>174</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -1564,7 +3550,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -1572,7 +3558,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -1580,7 +3566,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -1588,7 +3574,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -1596,7 +3582,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -1604,7 +3590,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -1612,7 +3598,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -1620,7 +3606,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>100</v>
+        <v>170</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -1628,7 +3614,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>101</v>
+        <v>61</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -1636,7 +3622,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>102</v>
+        <v>32</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -1644,7 +3630,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>103</v>
+        <v>171</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -1652,7 +3638,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>104</v>
+        <v>152</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -1660,7 +3646,862 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>105</v>
+        <v>112</v>
+      </c>
+      <c r="B105">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6972F11A-3BD3-4C6A-BE5F-2C656836A2F9}">
+  <dimension ref="A1:B138"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B15">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18">
+        <v>999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>203</v>
+      </c>
+      <c r="B40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>183</v>
+      </c>
+      <c r="B45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>186</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>187</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>188</v>
+      </c>
+      <c r="B51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>209</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>172</v>
+      </c>
+      <c r="B53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>189</v>
+      </c>
+      <c r="B55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>190</v>
+      </c>
+      <c r="B57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>199</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>84</v>
+      </c>
+      <c r="B59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>184</v>
+      </c>
+      <c r="B60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>204</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>147</v>
+      </c>
+      <c r="B62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>175</v>
+      </c>
+      <c r="B65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>16</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>179</v>
+      </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>191</v>
+      </c>
+      <c r="B70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>43</v>
+      </c>
+      <c r="B71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>156</v>
+      </c>
+      <c r="B73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>164</v>
+      </c>
+      <c r="B74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>86</v>
+      </c>
+      <c r="B76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>132</v>
+      </c>
+      <c r="B77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>205</v>
+      </c>
+      <c r="B78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>192</v>
+      </c>
+      <c r="B79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>148</v>
+      </c>
+      <c r="B80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>212</v>
+      </c>
+      <c r="B81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>58</v>
+      </c>
+      <c r="B82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>93</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>200</v>
+      </c>
+      <c r="B84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>107</v>
+      </c>
+      <c r="B85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>149</v>
+      </c>
+      <c r="B86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>23</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>151</v>
+      </c>
+      <c r="B88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>210</v>
+      </c>
+      <c r="B89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>106</v>
+      </c>
+      <c r="B90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>63</v>
+      </c>
+      <c r="B92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>193</v>
+      </c>
+      <c r="B93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>194</v>
+      </c>
+      <c r="B94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>81</v>
+      </c>
+      <c r="B96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>158</v>
+      </c>
+      <c r="B97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>48</v>
+      </c>
+      <c r="B98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>201</v>
+      </c>
+      <c r="B99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>94</v>
+      </c>
+      <c r="B100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>74</v>
+      </c>
+      <c r="B101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>88</v>
+      </c>
+      <c r="B102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>195</v>
+      </c>
+      <c r="B103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>143</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>14</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -1668,7 +4509,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>106</v>
+        <v>157</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -1676,7 +4517,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>206</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -1684,7 +4525,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -1692,7 +4533,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>109</v>
+        <v>202</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -1700,7 +4541,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>110</v>
+        <v>196</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -1708,7 +4549,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>111</v>
+        <v>211</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -1716,7 +4557,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>112</v>
+        <v>170</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -1724,7 +4565,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>113</v>
+        <v>50</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -1732,7 +4573,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>114</v>
+        <v>144</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -1740,7 +4581,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>115</v>
+        <v>18</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -1748,7 +4589,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>116</v>
+        <v>207</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -1756,7 +4597,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>117</v>
+        <v>19</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -1764,7 +4605,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>118</v>
+        <v>213</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -1772,7 +4613,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -1780,7 +4621,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -1788,7 +4629,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>121</v>
+        <v>160</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -1796,7 +4637,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>122</v>
+        <v>89</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -1804,7 +4645,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -1812,7 +4653,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>124</v>
+        <v>208</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -1820,7 +4661,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>125</v>
+        <v>60</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -1828,7 +4669,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -1836,7 +4677,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -1844,7 +4685,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>128</v>
+        <v>69</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -1852,7 +4693,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>129</v>
+        <v>185</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -1860,7 +4701,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -1868,7 +4709,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>131</v>
+        <v>197</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -1876,7 +4717,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -1884,7 +4725,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -1892,7 +4733,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -1900,7 +4741,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>135</v>
+        <v>198</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -1908,7 +4749,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>136</v>
+        <v>98</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -1916,7 +4757,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>137</v>
+        <v>43</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -1924,17 +4765,9 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="B138">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" t="s">
-        <v>139</v>
-      </c>
-      <c r="B139">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FIX] some model adjustments (e.g. iCC651); Models identifiers
</commit_message>
<xml_diff>
--- a/environmental_conditions/carbon_sources_conditions.xlsx
+++ b/environmental_conditions/carbon_sources_conditions.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Pycharm_projects/lab_models/environmental_conditions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="169" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FC362CC8-8313-447E-BF99-0741F437D713}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C8ACB19-7822-493D-8A37-E7B1FA126C29}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-96" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
   </bookViews>
   <sheets>
-    <sheet name="iCC390" sheetId="2" r:id="rId1"/>
+    <sheet name="iCC389" sheetId="2" r:id="rId1"/>
     <sheet name="iCC431" sheetId="1" r:id="rId2"/>
-    <sheet name="iCC464" sheetId="3" r:id="rId3"/>
-    <sheet name="iCC644" sheetId="4" r:id="rId4"/>
+    <sheet name="iCC470" sheetId="3" r:id="rId3"/>
+    <sheet name="iCC651" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iCC464'!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'iCC470'!$A$1:$B$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="214">
   <si>
     <t>exchange</t>
   </si>
@@ -1045,8 +1045,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05448E04-8BCE-4735-A6A7-A6D273D113C3}">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,7 +1165,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1341,7 +1341,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1685,7 +1685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F2E160-0E44-4C80-A334-F20DED143A47}">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -2816,8 +2816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1127718F-E99E-4924-AB7E-48BFF007017E}">
   <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3685,10 +3685,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6972F11A-3BD3-4C6A-BE5F-2C656836A2F9}">
-  <dimension ref="A1:B138"/>
+  <dimension ref="A1:B139"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4287,7 +4287,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -4295,7 +4295,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>86</v>
+        <v>155</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -4303,7 +4303,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -4311,7 +4311,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>205</v>
+        <v>132</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -4319,7 +4319,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -4327,7 +4327,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>148</v>
+        <v>192</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -4335,7 +4335,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>212</v>
+        <v>148</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -4343,7 +4343,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>58</v>
+        <v>212</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -4351,7 +4351,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>93</v>
+        <v>58</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -4359,7 +4359,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>200</v>
+        <v>93</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -4367,7 +4367,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>107</v>
+        <v>200</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -4375,7 +4375,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>149</v>
+        <v>107</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -4383,7 +4383,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>23</v>
+        <v>149</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -4391,7 +4391,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>151</v>
+        <v>23</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -4399,7 +4399,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>210</v>
+        <v>151</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -4407,7 +4407,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>106</v>
+        <v>210</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -4415,7 +4415,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -4423,7 +4423,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -4431,7 +4431,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>193</v>
+        <v>63</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -4439,7 +4439,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -4447,7 +4447,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -4455,7 +4455,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -4463,7 +4463,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>158</v>
+        <v>81</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -4471,7 +4471,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>48</v>
+        <v>158</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -4479,7 +4479,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>201</v>
+        <v>48</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -4487,7 +4487,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>94</v>
+        <v>201</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -4495,7 +4495,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -4503,7 +4503,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -4511,7 +4511,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>195</v>
+        <v>88</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -4519,7 +4519,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>143</v>
+        <v>195</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -4527,7 +4527,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -4535,7 +4535,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>157</v>
+        <v>14</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -4543,7 +4543,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>206</v>
+        <v>157</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -4551,7 +4551,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>122</v>
+        <v>206</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -4559,7 +4559,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -4567,7 +4567,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -4583,7 +4583,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>170</v>
+        <v>211</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -4591,7 +4591,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>50</v>
+        <v>170</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -4599,7 +4599,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>144</v>
+        <v>50</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -4607,7 +4607,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>18</v>
+        <v>144</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -4615,7 +4615,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>207</v>
+        <v>18</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -4623,7 +4623,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>19</v>
+        <v>207</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>213</v>
+        <v>19</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -4639,7 +4639,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>49</v>
+        <v>213</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -4647,7 +4647,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -4655,7 +4655,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>160</v>
+        <v>61</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -4663,7 +4663,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>89</v>
+        <v>160</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -4671,7 +4671,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -4679,7 +4679,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>208</v>
+        <v>45</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -4687,7 +4687,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>60</v>
+        <v>208</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -4695,7 +4695,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>153</v>
+        <v>60</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -4703,7 +4703,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -4711,7 +4711,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>69</v>
+        <v>150</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -4719,7 +4719,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>185</v>
+        <v>69</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -4727,7 +4727,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>154</v>
+        <v>185</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -4735,7 +4735,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -4743,7 +4743,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>112</v>
+        <v>197</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -4751,7 +4751,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>169</v>
+        <v>112</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -4759,7 +4759,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -4767,7 +4767,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>198</v>
+        <v>152</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -4775,7 +4775,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>98</v>
+        <v>198</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -4783,7 +4783,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>43</v>
+        <v>98</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -4791,9 +4791,17 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
+        <v>43</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A139" t="s">
         <v>54</v>
       </c>
-      <c r="B138">
+      <c r="B139">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FIX] lr growth, glucose and amino acids consumption rates
</commit_message>
<xml_diff>
--- a/environmental_conditions/carbon_sources_conditions.xlsx
+++ b/environmental_conditions/carbon_sources_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Pycharm_projects/lab_models/environmental_conditions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="185" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4C8ACB19-7822-493D-8A37-E7B1FA126C29}"/>
+  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3D44DA87-BD9B-45D1-B225-770E8D7188B9}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
   </bookViews>
   <sheets>
     <sheet name="iCC389" sheetId="2" r:id="rId1"/>
@@ -1045,7 +1045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05448E04-8BCE-4735-A6A7-A6D273D113C3}">
   <dimension ref="A1:B78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -3687,8 +3687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6972F11A-3BD3-4C6A-BE5F-2C656836A2F9}">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3847,7 +3847,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -3855,7 +3855,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -3863,15 +3863,15 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>0.14199999999999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>36</v>
       </c>
       <c r="B23">
         <v>1</v>
@@ -3879,23 +3879,23 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B24">
-        <v>1</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B25">
-        <v>1</v>
+        <v>0.17599999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>139</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -3903,7 +3903,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B27">
         <v>1</v>
@@ -3911,7 +3911,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B28">
         <v>1</v>
@@ -3919,7 +3919,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -3927,7 +3927,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="B30">
         <v>1</v>
@@ -3935,7 +3935,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -3943,7 +3943,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -3951,7 +3951,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -3959,7 +3959,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B34">
         <v>1</v>
@@ -3967,15 +3967,15 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B35">
-        <v>1</v>
+        <v>0.17799999999999999</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -3983,7 +3983,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -3991,7 +3991,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B38">
         <v>1</v>

</xml_diff>

<commit_message>
[FIX] carbon source uniformization; Lh using glucose [ADD] memote validation
</commit_message>
<xml_diff>
--- a/environmental_conditions/carbon_sources_conditions.xlsx
+++ b/environmental_conditions/carbon_sources_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uminho365-my.sharepoint.com/personal/id8006_uminho_pt/Documents/Pycharm_projects/lab_models/environmental_conditions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="187" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3D44DA87-BD9B-45D1-B225-770E8D7188B9}"/>
+  <xr:revisionPtr revIDLastSave="194" documentId="13_ncr:1_{FCA6B269-E553-4911-B379-7AAEED1BFC5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D537E072-96A8-402B-A4AD-056D69D12929}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{49D59947-69D5-4711-8775-965F805B02F1}"/>
   </bookViews>
   <sheets>
     <sheet name="iCC389" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="213">
   <si>
     <t>exchange</t>
   </si>
@@ -553,9 +553,6 @@
   </si>
   <si>
     <t>EX_acmum_e</t>
-  </si>
-  <si>
-    <t>EX_C16639_e</t>
   </si>
   <si>
     <t>EX_melib_e</t>
@@ -1043,10 +1040,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05448E04-8BCE-4735-A6A7-A6D273D113C3}">
-  <dimension ref="A1:B78"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1165,7 +1162,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1341,7 +1338,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -1664,14 +1661,6 @@
         <v>112</v>
       </c>
       <c r="B77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>61</v>
-      </c>
-      <c r="B78">
         <v>0</v>
       </c>
     </row>
@@ -2816,8 +2805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1127718F-E99E-4924-AB7E-48BFF007017E}">
   <dimension ref="A1:B107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3176,7 +3165,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -3208,7 +3197,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -3240,7 +3229,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -3288,7 +3277,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -3304,7 +3293,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -3320,7 +3309,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -3344,7 +3333,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -3512,7 +3501,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -3544,7 +3533,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -3560,7 +3549,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -3656,7 +3645,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>171</v>
+        <v>152</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -3664,7 +3653,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>152</v>
+        <v>112</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -3672,7 +3661,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -3687,7 +3676,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6972F11A-3BD3-4C6A-BE5F-2C656836A2F9}">
   <dimension ref="A1:B139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A125" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -3807,7 +3796,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B15">
         <v>999999</v>
@@ -4007,7 +3996,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -4047,7 +4036,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -4063,7 +4052,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B47">
         <v>0</v>
@@ -4079,7 +4068,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -4095,7 +4084,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -4103,7 +4092,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -4111,7 +4100,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -4127,7 +4116,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -4143,7 +4132,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -4151,7 +4140,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -4167,7 +4156,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -4175,7 +4164,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -4207,7 +4196,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -4239,7 +4228,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -4247,7 +4236,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B70">
         <v>0</v>
@@ -4319,7 +4308,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -4327,7 +4316,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -4343,7 +4332,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -4367,7 +4356,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -4407,7 +4396,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -4439,7 +4428,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -4447,7 +4436,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -4487,7 +4476,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -4519,7 +4508,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B104">
         <v>0</v>
@@ -4551,7 +4540,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -4567,7 +4556,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -4575,7 +4564,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -4583,7 +4572,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -4623,7 +4612,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -4639,7 +4628,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -4687,7 +4676,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -4727,7 +4716,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -4743,7 +4732,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -4775,7 +4764,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B136">
         <v>0</v>

</xml_diff>